<commit_message>
adding to excluding criterium sdrr<200
</commit_message>
<xml_diff>
--- a/RSA analysis/All excluded subs.xlsx
+++ b/RSA analysis/All excluded subs.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,89 +439,310 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sub_id (25 subs)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_0 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_0 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_0 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_2 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Session length (53.12s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Session length (59.89s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Long IBI count (56) exceeds 20% of series length (204)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SDRR (3329.97) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SDRR (637.07) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SDRR (855.91) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SDRR (3248.83) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Unmatched subject</t>
         </is>
@@ -538,7 +759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,89 +770,310 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sub_id (25 subs)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_1 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Session length (53.33s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Long IBI count (27) exceeds 20% of series length (120)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SDRR (234.48) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SDRR (1134.84) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SDRR (528.73) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SDRR (912.60) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SDRR (207.60) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SDRR (256.63) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SDRR (1194.80) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SDRR (214.04) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SDRR (236.40) exceeds threshold (200)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SDRR (473.00) exceeds threshold (200)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Unmatched subject</t>
         </is>
@@ -648,7 +1090,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,159 +1101,418 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sub_id (34 subs)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_1 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_2 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_2 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_2 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Session length (33.63s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Session length (36.64s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Session length (57.19s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Session length (51.12s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Session length (15.99s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Session length (33.91s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Session length (22.91s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Session length (54.37s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Session length (49.27s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Session length (41.50s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Session length (52.73s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Long IBI count (34) exceeds 20% of series length (72)</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Long IBI count (31) exceeds 20% of series length (65)</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Long IBI count (43) exceeds 20% of series length (99)</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SDRR (307.23) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SDRR (1343.10) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SDRR (355.55) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Unmatched subject</t>
         </is>
@@ -828,7 +1529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,159 +1540,418 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>sub_id (34 subs)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>IBI data for best channel ch_2 does not match peak differences</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Session length (33.84s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Session length (36.69s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Session length (37.29s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Session length (57.19s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Session length (51.06s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Session length (34.01s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Session length (31.92s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Session length (22.52s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Session length (54.23s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Session length (41.86s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Session length (52.25s) is shorter than 60 sec</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Long IBI count (10) exceeds 20% of series length (39)</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SDRR (240.87) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SDRR (210.78) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SDRR (441.76) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SDRR (329.50) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SDRR (384.76) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SDRR (227.95) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SDRR (300.59) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Unmatched subject</t>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SDRR (332.77) exceeds threshold (200)</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SDRR (471.06) exceeds threshold (200)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SDRR (375.08) exceeds threshold (200)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Unmatched subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Unmatched subject</t>
         </is>

</xml_diff>

<commit_message>
creating ibi interpolation pipeline
</commit_message>
<xml_diff>
--- a/RSA analysis/All excluded subs.xlsx
+++ b/RSA analysis/All excluded subs.xlsx
@@ -583,7 +583,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -595,7 +595,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -607,7 +607,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -619,7 +619,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -631,7 +631,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -643,7 +643,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -655,7 +655,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -667,7 +667,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>86</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -679,7 +679,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>85</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -703,7 +703,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>02</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -715,7 +715,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -727,7 +727,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -739,7 +739,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>76</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -950,7 +950,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -974,7 +974,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>68</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -986,7 +986,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1010,7 +1010,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1022,7 +1022,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1034,7 +1034,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1046,7 +1046,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1070,7 +1070,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1365,7 +1365,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1401,7 +1401,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1413,7 +1413,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1425,7 +1425,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1437,7 +1437,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1449,7 +1449,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1461,7 +1461,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1473,7 +1473,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>57</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1485,7 +1485,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1497,7 +1497,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>02</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1509,7 +1509,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1876,7 +1876,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1888,7 +1888,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1900,7 +1900,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>77</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>87</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1936,7 +1936,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>88</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1948,7 +1948,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">

</xml_diff>